<commit_message>
cambios en arca. correcciones
</commit_message>
<xml_diff>
--- a/Capitulo999_CORRECCIONES/COHORTE03/EvaluacionTP05.xlsx
+++ b/Capitulo999_CORRECCIONES/COHORTE03/EvaluacionTP05.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF0FA18-3619-4757-B9B0-4893F73A7104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D3058C-3615-4984-91B2-570852DDDCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="2940" windowWidth="21600" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$47</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="150">
   <si>
     <t>VILLEGAS AUGUSTO</t>
   </si>
@@ -380,6 +383,96 @@
   </si>
   <si>
     <t>CRISTIAN AGUSTIN</t>
+  </si>
+  <si>
+    <t>MOMBELLI, ANTONELLA MAGALI</t>
+  </si>
+  <si>
+    <t>MOMBELLI</t>
+  </si>
+  <si>
+    <t>ANTONELLA MAGALI</t>
+  </si>
+  <si>
+    <t>OLMEDO, FRANCO SIMON</t>
+  </si>
+  <si>
+    <t>OLMEDO</t>
+  </si>
+  <si>
+    <t>FRANCO SIMON</t>
+  </si>
+  <si>
+    <t>ROJAS, JUAN ANDRES</t>
+  </si>
+  <si>
+    <t>ROJAS</t>
+  </si>
+  <si>
+    <t>JUAN ANDRES</t>
+  </si>
+  <si>
+    <t>VEGA, NANCY BEATRIZ</t>
+  </si>
+  <si>
+    <t>VEGA</t>
+  </si>
+  <si>
+    <t>NANCY BEATRIZ</t>
+  </si>
+  <si>
+    <t>COPIADO</t>
+  </si>
+  <si>
+    <t>LUNA, MARIA EUGENIA</t>
+  </si>
+  <si>
+    <t>LUNA</t>
+  </si>
+  <si>
+    <t>MARIA EUGENIA</t>
+  </si>
+  <si>
+    <t>QUINTEROS, GABINO MIGUEL</t>
+  </si>
+  <si>
+    <t>QUINTEROS</t>
+  </si>
+  <si>
+    <t>GABINO MIGUEL</t>
+  </si>
+  <si>
+    <t>CISTERNA, GASTÓN MAXIMILIANO</t>
+  </si>
+  <si>
+    <t>CISTERNA</t>
+  </si>
+  <si>
+    <t>GASTÓN MAXIMILIANO</t>
+  </si>
+  <si>
+    <t>CONCILIADO</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>ENLACE</t>
+  </si>
+  <si>
+    <t>Proyecto vacío. Sin nada</t>
+  </si>
+  <si>
+    <t>PASADO A PLANILLA ?.</t>
+  </si>
+  <si>
+    <t>No tiene los trabajos anteriores presentados</t>
+  </si>
+  <si>
+    <t>DUPLICADA</t>
+  </si>
+  <si>
+    <t>Posible copia</t>
   </si>
 </sst>
 </file>
@@ -397,24 +490,18 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -425,6 +512,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF227ACB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,12 +546,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,704 +841,1234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F40"/>
+  <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>57</v>
       </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>60</v>
       </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>62</v>
       </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" t="s">
         <v>65</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>64</v>
       </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>86</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>85</v>
       </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" t="s">
         <v>84</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>83</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>82</v>
       </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" t="s">
         <v>80</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>79</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>78</v>
       </c>
-      <c r="E28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" t="s">
         <v>77</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>76</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>75</v>
       </c>
-      <c r="E29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>73</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>72</v>
       </c>
-      <c r="E30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
         <v>71</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>70</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>69</v>
       </c>
-      <c r="E31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>67</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>66</v>
       </c>
-      <c r="E32" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>95</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="E33" t="s">
-        <v>1</v>
-      </c>
       <c r="F33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2</v>
+      </c>
+      <c r="H33" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>98</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>99</v>
       </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
       <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" t="s">
         <v>101</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>102</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>103</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>104</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" s="5">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" t="s">
         <v>105</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>106</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>107</v>
       </c>
-      <c r="E36" t="s">
-        <v>1</v>
-      </c>
       <c r="F36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2</v>
+      </c>
+      <c r="H36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" t="s">
         <v>109</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>108</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>110</v>
       </c>
-      <c r="E37" t="s">
-        <v>1</v>
-      </c>
       <c r="F37" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>112</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>113</v>
       </c>
-      <c r="E38" t="s">
-        <v>1</v>
-      </c>
       <c r="F38" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" t="s">
         <v>114</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>115</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>116</v>
       </c>
-      <c r="E39" t="s">
-        <v>1</v>
-      </c>
       <c r="F39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5">
+        <v>2</v>
+      </c>
+      <c r="H39" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E40" t="s">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="F40" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="5">
+        <v>2</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G41" s="5">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <v>2</v>
+      </c>
+      <c r="H42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" t="s">
+        <v>128</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="5">
+        <v>2</v>
+      </c>
+      <c r="H43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>42</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G44" s="5">
+        <v>2</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5">
+        <v>2</v>
+      </c>
+      <c r="H45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="5">
+        <v>2</v>
+      </c>
+      <c r="H46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5">
+        <v>2</v>
+      </c>
+      <c r="H47" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A2:H47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>